<commit_message>
memoria 4 a falta de medidas
</commit_message>
<xml_diff>
--- a/Practica 4/Libro1.xlsx
+++ b/Practica 4/Libro1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eps\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nacho\CIREL\Practica 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>frecuencia (Hz)</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Grados (º)</t>
+  </si>
+  <si>
+    <t>Circuito 10K y 22K</t>
   </si>
 </sst>
 </file>
@@ -334,11 +337,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="264421696"/>
-        <c:axId val="264423376"/>
+        <c:axId val="198896952"/>
+        <c:axId val="198897736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="264421696"/>
+        <c:axId val="198896952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -451,12 +454,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="264423376"/>
+        <c:crossAx val="198897736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="264423376"/>
+        <c:axId val="198897736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -574,7 +577,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="264421696"/>
+        <c:crossAx val="198896952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -832,11 +835,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="222210960"/>
-        <c:axId val="262477072"/>
+        <c:axId val="198898520"/>
+        <c:axId val="198895384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="222210960"/>
+        <c:axId val="198898520"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -952,12 +955,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262477072"/>
+        <c:crossAx val="198895384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="262477072"/>
+        <c:axId val="198895384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1075,7 +1078,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222210960"/>
+        <c:crossAx val="198898520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1338,11 +1341,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="265978624"/>
-        <c:axId val="267712688"/>
+        <c:axId val="198892640"/>
+        <c:axId val="198899304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="265978624"/>
+        <c:axId val="198892640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1455,12 +1458,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="267712688"/>
+        <c:crossAx val="198899304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="267712688"/>
+        <c:axId val="198899304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1573,7 +1576,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="265978624"/>
+        <c:crossAx val="198892640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1836,11 +1839,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="265977504"/>
-        <c:axId val="262195344"/>
+        <c:axId val="198891856"/>
+        <c:axId val="198892248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="265977504"/>
+        <c:axId val="198891856"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1956,12 +1959,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262195344"/>
+        <c:crossAx val="198892248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="262195344"/>
+        <c:axId val="198892248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2074,7 +2077,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="265977504"/>
+        <c:crossAx val="198891856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2337,11 +2340,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115576816"/>
-        <c:axId val="115577376"/>
+        <c:axId val="198896168"/>
+        <c:axId val="198896560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115576816"/>
+        <c:axId val="198896168"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2462,12 +2465,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115577376"/>
+        <c:crossAx val="198896560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115577376"/>
+        <c:axId val="198896560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2580,7 +2583,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115576816"/>
+        <c:crossAx val="198896168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2838,11 +2841,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218615568"/>
-        <c:axId val="218616688"/>
+        <c:axId val="198893816"/>
+        <c:axId val="198894600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218615568"/>
+        <c:axId val="198893816"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2958,12 +2961,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218616688"/>
+        <c:crossAx val="198894600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218616688"/>
+        <c:axId val="198894600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3076,7 +3079,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218615568"/>
+        <c:crossAx val="198893816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6911,8 +6914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6939,6 +6942,15 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="3"/>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -7874,8 +7886,9 @@
       <c r="M30" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="I1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>